<commit_message>
Correction English spell for modelling
</commit_message>
<xml_diff>
--- a/public/directory/members2.xlsx
+++ b/public/directory/members2.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="138">
   <si>
     <t>first_name</t>
   </si>
@@ -391,9 +391,6 @@
   </si>
   <si>
     <t>Thompson</t>
-  </si>
-  <si>
-    <t>modelling</t>
   </si>
   <si>
     <t>University of Oxford</t>
@@ -444,7 +441,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00000"/>
-    <numFmt numFmtId="166" formatCode="###0.0000"/>
+    <numFmt numFmtId="165" formatCode="###0.0000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -530,25 +527,25 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -891,7 +888,7 @@
   <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -945,10 +942,10 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>10</v>
@@ -1382,13 +1379,13 @@
     </row>
     <row r="8" spans="1:22" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>95</v>
@@ -1418,16 +1415,16 @@
         <v>0.43830000000000002</v>
       </c>
       <c r="M8" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="P8" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>136</v>
       </c>
       <c r="Q8" s="1" t="s">
         <v>34</v>
@@ -1462,19 +1459,19 @@
         <v>95</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>124</v>
+        <v>43</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>79</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>88</v>
@@ -1486,13 +1483,13 @@
         <v>-1.255522</v>
       </c>
       <c r="M9" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="N9" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="N9" s="2" t="s">
+      <c r="O9" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="Q9" s="1" t="s">
         <v>34</v>

</xml_diff>